<commit_message>
Added the learning results of the new model and added code to evaluate the learned model.
</commit_message>
<xml_diff>
--- a/model_information/Performance By Model.xlsx
+++ b/model_information/Performance By Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyun\Desktop\RecycleWasteClassifier\model_information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C89C98-9B10-461F-AD26-6CFE28D6FCBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801D208A-4765-4A8E-B293-DB67A269CCDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4530" yWindow="1080" windowWidth="17025" windowHeight="12930" xr2:uid="{3D546535-CEB8-4C73-9D93-428EFDA1FC9D}"/>
   </bookViews>
@@ -540,7 +540,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -751,8 +751,12 @@
       <c r="D10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="E10" s="2">
+        <v>0.4214</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.85099999999999998</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">

</xml_diff>

<commit_message>
Saved the output for the model and modified the code.
</commit_message>
<xml_diff>
--- a/model_information/Performance By Model.xlsx
+++ b/model_information/Performance By Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyun\Desktop\RecycleWasteClassifier\model_information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801D208A-4765-4A8E-B293-DB67A269CCDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6B4202-24FE-4955-A07A-488D1C3BD456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4530" yWindow="1080" windowWidth="17025" windowHeight="12930" xr2:uid="{3D546535-CEB8-4C73-9D93-428EFDA1FC9D}"/>
   </bookViews>
@@ -540,7 +540,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -771,8 +771,12 @@
       <c r="D11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="E11" s="2">
+        <v>0.34549999999999997</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.88270000000000004</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Several code fixes were made.
</commit_message>
<xml_diff>
--- a/model_information/Performance By Model.xlsx
+++ b/model_information/Performance By Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyun\Desktop\RecycleWasteClassifier\model_information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6B4202-24FE-4955-A07A-488D1C3BD456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD8548B-78EB-48C6-AEFD-035766B10F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4530" yWindow="1080" windowWidth="17025" windowHeight="12930" xr2:uid="{3D546535-CEB8-4C73-9D93-428EFDA1FC9D}"/>
+    <workbookView xWindow="6885" yWindow="1650" windowWidth="17025" windowHeight="12930" xr2:uid="{3D546535-CEB8-4C73-9D93-428EFDA1FC9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
The models were retrained.
</commit_message>
<xml_diff>
--- a/model_information/Performance By Model.xlsx
+++ b/model_information/Performance By Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyun\Desktop\RecycleWasteClassifier\model_information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD8548B-78EB-48C6-AEFD-035766B10F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50E565F-E638-4B27-8DAD-90288E8D442D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6885" yWindow="1650" windowWidth="17025" windowHeight="12930" xr2:uid="{3D546535-CEB8-4C73-9D93-428EFDA1FC9D}"/>
+    <workbookView xWindow="5070" yWindow="1665" windowWidth="17025" windowHeight="12930" xr2:uid="{3D546535-CEB8-4C73-9D93-428EFDA1FC9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -540,7 +540,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -592,7 +592,7 @@
         <v>15</v>
       </c>
       <c r="E2" s="2">
-        <v>0.64459999999999995</v>
+        <v>0.6542</v>
       </c>
       <c r="F2" s="2">
         <v>0.75</v>
@@ -612,10 +612,10 @@
         <v>16</v>
       </c>
       <c r="E3" s="2">
-        <v>0.49959999999999999</v>
+        <v>0.4798</v>
       </c>
       <c r="F3" s="2">
-        <v>0.81730000000000003</v>
+        <v>0.82210000000000005</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -632,10 +632,10 @@
         <v>17</v>
       </c>
       <c r="E4" s="2">
-        <v>0.45140000000000002</v>
+        <v>0.33489999999999998</v>
       </c>
       <c r="F4" s="2">
-        <v>0.84619999999999995</v>
+        <v>0.89810000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -651,12 +651,8 @@
       <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="2">
-        <v>0.45700000000000002</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.82789999999999997</v>
-      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -671,12 +667,8 @@
       <c r="D6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="2">
-        <v>0.40810000000000002</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.86439999999999995</v>
-      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -691,12 +683,8 @@
       <c r="D7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="2">
-        <v>0.4582</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0.82310000000000005</v>
-      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -711,12 +699,8 @@
       <c r="D8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="2">
-        <v>0.39789999999999998</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0.84040000000000004</v>
-      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -731,12 +715,8 @@
       <c r="D9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="2">
-        <v>0.44379999999999997</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0.83079999999999998</v>
-      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -751,12 +731,8 @@
       <c r="D10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="2">
-        <v>0.4214</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0.85099999999999998</v>
-      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -771,12 +747,8 @@
       <c r="D11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="2">
-        <v>0.34549999999999997</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0.88270000000000004</v>
-      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Most of the files were modified in general.
</commit_message>
<xml_diff>
--- a/model_information/Performance By Model.xlsx
+++ b/model_information/Performance By Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyun\Desktop\RecycleWasteClassifier\model_information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50E565F-E638-4B27-8DAD-90288E8D442D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75B7FDA-6370-4107-9047-E71085C9F2A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="1665" windowWidth="17025" windowHeight="12930" xr2:uid="{3D546535-CEB8-4C73-9D93-428EFDA1FC9D}"/>
+    <workbookView xWindow="7575" yWindow="2010" windowWidth="17025" windowHeight="12930" xr2:uid="{3D546535-CEB8-4C73-9D93-428EFDA1FC9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Accuracy</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -155,14 +155,6 @@
   </si>
   <si>
     <t>MobileNetV3(small)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Previous Accuracy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Previous Loss</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -537,218 +529,226 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFAB712-2674-4A68-BC93-213602476CB7}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>224</v>
-      </c>
-      <c r="C2" s="2" t="s">
+        <v>0.730934798717498</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.72554349899291903</v>
+      </c>
+      <c r="D2" s="2">
+        <v>224</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="2">
-        <v>0.6542</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2">
-        <v>224</v>
-      </c>
-      <c r="C3" s="2" t="s">
+        <v>0.52614372968673695</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.8125</v>
+      </c>
+      <c r="D3" s="2">
+        <v>224</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="2">
-        <v>0.4798</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.82210000000000005</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="2">
-        <v>224</v>
-      </c>
-      <c r="C4" s="2" t="s">
+        <v>0.40091994404792702</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.86865943670272805</v>
+      </c>
+      <c r="D4" s="2">
+        <v>224</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="2">
-        <v>0.33489999999999998</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.89810000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2">
-        <v>224</v>
-      </c>
-      <c r="C5" s="2" t="s">
+        <v>0.32090279459953303</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.89492756128311102</v>
+      </c>
+      <c r="D5" s="2">
+        <v>224</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>32</v>
       </c>
       <c r="B6" s="2">
-        <v>224</v>
-      </c>
-      <c r="C6" s="2" t="s">
+        <v>0.27091637253761203</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.90670287609100297</v>
+      </c>
+      <c r="D6" s="2">
+        <v>224</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="2">
-        <v>224</v>
-      </c>
-      <c r="C7" s="2" t="s">
+        <v>0.48250153660774198</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.816123187541961</v>
+      </c>
+      <c r="D7" s="2">
+        <v>224</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B8" s="2">
-        <v>224</v>
-      </c>
-      <c r="C8" s="2" t="s">
+        <v>0.295252114534378</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.90851449966430597</v>
+      </c>
+      <c r="D8" s="2">
+        <v>224</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="2">
-        <v>224</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2">
+        <v>224</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="2">
-        <v>224</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2">
+        <v>224</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="2">
-        <v>224</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2">
+        <v>224</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
The model was retrained and the code was slightly modified.
</commit_message>
<xml_diff>
--- a/model_information/Performance By Model.xlsx
+++ b/model_information/Performance By Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyun\Desktop\RecycleWasteClassifier\model_information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75B7FDA-6370-4107-9047-E71085C9F2A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5225CB49-AEBE-4AC2-8D50-E3AD0728BC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7575" yWindow="2010" windowWidth="17025" windowHeight="12930" xr2:uid="{3D546535-CEB8-4C73-9D93-428EFDA1FC9D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3D546535-CEB8-4C73-9D93-428EFDA1FC9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -166,6 +166,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="178" formatCode="0.000_ "/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -205,7 +208,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -213,6 +216,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -532,14 +538,15 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="5.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.75" bestFit="1" customWidth="1"/>
   </cols>
@@ -566,10 +573,10 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>0.730934798717498</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>0.72554349899291903</v>
       </c>
       <c r="D2" s="2">
@@ -586,10 +593,10 @@
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>0.52614372968673695</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>0.8125</v>
       </c>
       <c r="D3" s="2">
@@ -606,10 +613,10 @@
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>0.40091994404792702</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>0.86865943670272805</v>
       </c>
       <c r="D4" s="2">
@@ -626,10 +633,10 @@
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>0.32090279459953303</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <v>0.89492756128311102</v>
       </c>
       <c r="D5" s="2">
@@ -646,10 +653,10 @@
       <c r="A6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>0.27091637253761203</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>0.90670287609100297</v>
       </c>
       <c r="D6" s="2">
@@ -666,10 +673,10 @@
       <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <v>0.48250153660774198</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <v>0.816123187541961</v>
       </c>
       <c r="D7" s="2">
@@ -686,10 +693,10 @@
       <c r="A8" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="3">
         <v>0.295252114534378</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <v>0.90851449966430597</v>
       </c>
       <c r="D8" s="2">
@@ -706,8 +713,12 @@
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="B9" s="3">
+        <v>0.29797556996345498</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.90760868787765503</v>
+      </c>
       <c r="D9" s="2">
         <v>224</v>
       </c>
@@ -722,8 +733,12 @@
       <c r="A10" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="B10" s="3">
+        <v>0.41326564550399703</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.85778987407684304</v>
+      </c>
       <c r="D10" s="2">
         <v>224</v>
       </c>
@@ -738,8 +753,12 @@
       <c r="A11" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="B11" s="3">
+        <v>0.31138986349105802</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.91123187541961603</v>
+      </c>
       <c r="D11" s="2">
         <v>224</v>
       </c>

</xml_diff>

<commit_message>
The matplotlib code was modified.
</commit_message>
<xml_diff>
--- a/model_information/Performance By Model.xlsx
+++ b/model_information/Performance By Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyun\Desktop\RecycleWasteClassifier\model_information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5225CB49-AEBE-4AC2-8D50-E3AD0728BC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300929A7-8442-40EB-BEAF-D13A5B3F3912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3D546535-CEB8-4C73-9D93-428EFDA1FC9D}"/>
+    <workbookView xWindow="7575" yWindow="2010" windowWidth="17025" windowHeight="12930" xr2:uid="{3D546535-CEB8-4C73-9D93-428EFDA1FC9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -167,7 +167,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="0.000_ "/>
+    <numFmt numFmtId="176" formatCode="0.000_ "/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -208,17 +208,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -546,7 +543,7 @@
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.75" bestFit="1" customWidth="1"/>
   </cols>
@@ -565,207 +562,207 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>0.730934798717498</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>0.72554349899291903</v>
       </c>
-      <c r="D2" s="2">
-        <v>224</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="1">
+        <v>224</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>0.52614372968673695</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>0.8125</v>
       </c>
-      <c r="D3" s="2">
-        <v>224</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="1">
+        <v>224</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>0.40091994404792702</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>0.86865943670272805</v>
       </c>
-      <c r="D4" s="2">
-        <v>224</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="D4" s="1">
+        <v>224</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>0.32090279459953303</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>0.89492756128311102</v>
       </c>
-      <c r="D5" s="2">
-        <v>224</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="D5" s="1">
+        <v>224</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>0.27091637253761203</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>0.90670287609100297</v>
       </c>
-      <c r="D6" s="2">
-        <v>224</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="1">
+        <v>224</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>0.48250153660774198</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>0.816123187541961</v>
       </c>
-      <c r="D7" s="2">
-        <v>224</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="D7" s="1">
+        <v>224</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>0.295252114534378</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>0.90851449966430597</v>
       </c>
-      <c r="D8" s="2">
-        <v>224</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="D8" s="1">
+        <v>224</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>0.29797556996345498</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>0.90760868787765503</v>
       </c>
-      <c r="D9" s="2">
-        <v>224</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="D9" s="1">
+        <v>224</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>0.41326564550399703</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>0.85778987407684304</v>
       </c>
-      <c r="D10" s="2">
-        <v>224</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="D10" s="1">
+        <v>224</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>0.31138986349105802</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>0.91123187541961603</v>
       </c>
-      <c r="D11" s="2">
-        <v>224</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="D11" s="1">
+        <v>224</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="1" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
The type of training model was changed.
</commit_message>
<xml_diff>
--- a/model_information/Performance By Model.xlsx
+++ b/model_information/Performance By Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyun\Desktop\RecycleWasteClassifier\model_information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300929A7-8442-40EB-BEAF-D13A5B3F3912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE60DFD-23C2-4CFB-B9E8-3B39FC5BC860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7575" yWindow="2010" windowWidth="17025" windowHeight="12930" xr2:uid="{3D546535-CEB8-4C73-9D93-428EFDA1FC9D}"/>
+    <workbookView xWindow="6480" yWindow="1170" windowWidth="17025" windowHeight="12930" xr2:uid="{3D546535-CEB8-4C73-9D93-428EFDA1FC9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Accuracy</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -39,14 +39,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0.5M</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Size</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Input</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -55,38 +47,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3.5M</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MobileNet(alpha=0.50)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.3M</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MobileNetV2(alpha=0.35)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.7M</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MobileNetV2(alpha=0.50)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2.0M</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0.2M</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -103,10 +75,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2.6M</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0.9M</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -119,10 +87,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2.7M</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1.4M</t>
   </si>
   <si>
@@ -134,31 +98,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4.3M</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>3.2M</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>EfficientNet-B0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.3M</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.0M</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MobileNetV3(small)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>MobileNetV2(alpha=0.75)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parameters</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MobileNetV3(large)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.0M</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -532,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFAB712-2674-4A68-BC93-213602476CB7}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -544,11 +504,11 @@
     <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -557,16 +517,13 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -580,41 +537,35 @@
         <v>224</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2">
-        <v>0.52614372968673695</v>
+        <v>0.40091994404792702</v>
       </c>
       <c r="C3" s="2">
-        <v>0.8125</v>
+        <v>0.86865943670272805</v>
       </c>
       <c r="D3" s="1">
         <v>224</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2">
-        <v>0.40091994404792702</v>
+        <v>0.32090279459953303</v>
       </c>
       <c r="C4" s="2">
-        <v>0.86865943670272805</v>
+        <v>0.89492756128311102</v>
       </c>
       <c r="D4" s="1">
         <v>224</v>
@@ -622,33 +573,27 @@
       <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>0.32090279459953303</v>
+        <v>0.52614372968673695</v>
       </c>
       <c r="C5" s="2">
-        <v>0.89492756128311102</v>
+        <v>0.8125</v>
       </c>
       <c r="D5" s="1">
         <v>224</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2">
         <v>0.27091637253761203</v>
@@ -660,55 +605,46 @@
         <v>224</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="B7" s="2">
+        <v>0.295252114534378</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.90851449966430597</v>
+      </c>
+      <c r="D7" s="1">
+        <v>224</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2">
         <v>0.48250153660774198</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C8" s="2">
         <v>0.816123187541961</v>
       </c>
-      <c r="D7" s="1">
-        <v>224</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0.295252114534378</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.90851449966430597</v>
-      </c>
       <c r="D8" s="1">
         <v>224</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B9" s="2">
         <v>0.29797556996345498</v>
@@ -720,51 +656,48 @@
         <v>224</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="2">
+        <v>22</v>
+      </c>
+      <c r="D10" s="1">
+        <v>224</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2">
         <v>0.41326564550399703</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C11" s="2">
         <v>0.85778987407684304</v>
       </c>
-      <c r="D10" s="1">
-        <v>224</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="2">
-        <v>0.31138986349105802</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0.91123187541961603</v>
-      </c>
       <c r="D11" s="1">
         <v>224</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>31</v>
-      </c>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Prepared to train the model anew.
</commit_message>
<xml_diff>
--- a/model_information/Performance By Model.xlsx
+++ b/model_information/Performance By Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyun\Desktop\RecycleWasteClassifier\model_information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE60DFD-23C2-4CFB-B9E8-3B39FC5BC860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE90388D-8501-47FA-BD63-BF4832EE18E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6480" yWindow="1170" windowWidth="17025" windowHeight="12930" xr2:uid="{3D546535-CEB8-4C73-9D93-428EFDA1FC9D}"/>
   </bookViews>
@@ -527,12 +527,8 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
-        <v>0.730934798717498</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0.72554349899291903</v>
-      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
       <c r="D2" s="1">
         <v>224</v>
       </c>
@@ -544,12 +540,8 @@
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2">
-        <v>0.40091994404792702</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.86865943670272805</v>
-      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
       <c r="D3" s="1">
         <v>224</v>
       </c>
@@ -561,12 +553,8 @@
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2">
-        <v>0.32090279459953303</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.89492756128311102</v>
-      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
       <c r="D4" s="1">
         <v>224</v>
       </c>
@@ -578,12 +566,8 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2">
-        <v>0.52614372968673695</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.8125</v>
-      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
       <c r="D5" s="1">
         <v>224</v>
       </c>
@@ -595,12 +579,8 @@
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="2">
-        <v>0.27091637253761203</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0.90670287609100297</v>
-      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
       <c r="D6" s="1">
         <v>224</v>
       </c>
@@ -612,12 +592,8 @@
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="2">
-        <v>0.295252114534378</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0.90851449966430597</v>
-      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
       <c r="D7" s="1">
         <v>224</v>
       </c>
@@ -629,12 +605,8 @@
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2">
-        <v>0.48250153660774198</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.816123187541961</v>
-      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
       <c r="D8" s="1">
         <v>224</v>
       </c>
@@ -646,12 +618,8 @@
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="2">
-        <v>0.29797556996345498</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.90760868787765503</v>
-      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="1">
         <v>224</v>
       </c>
@@ -674,12 +642,8 @@
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="2">
-        <v>0.41326564550399703</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0.85778987407684304</v>
-      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
       <c r="D11" s="1">
         <v>224</v>
       </c>

</xml_diff>

<commit_message>
MobileNetV3 (large) was selected.
</commit_message>
<xml_diff>
--- a/model_information/Performance By Model.xlsx
+++ b/model_information/Performance By Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyun\Desktop\RecycleWasteClassifier\model_information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE90388D-8501-47FA-BD63-BF4832EE18E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B061018-30D4-41F9-94D6-D88E0DC69AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6480" yWindow="1170" windowWidth="17025" windowHeight="12930" xr2:uid="{3D546535-CEB8-4C73-9D93-428EFDA1FC9D}"/>
+    <workbookView xWindow="7065" yWindow="1380" windowWidth="17025" windowHeight="12930" xr2:uid="{3D546535-CEB8-4C73-9D93-428EFDA1FC9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -126,8 +126,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.000_ "/>
+    <numFmt numFmtId="178" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -168,7 +169,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -177,6 +178,9 @@
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -501,7 +505,7 @@
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
@@ -509,145 +513,186 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="1">
-        <v>224</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="B2" s="3">
+        <v>0.73988103866577104</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.72463768720626798</v>
+      </c>
+      <c r="D2">
+        <v>224</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="1">
-        <v>224</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="B3" s="3">
+        <v>0.45119205117225603</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.84601449966430597</v>
+      </c>
+      <c r="D3">
+        <v>224</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="1">
-        <v>224</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="B4" s="3">
+        <v>0.33470913767814597</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.88949275016784601</v>
+      </c>
+      <c r="D4">
+        <v>224</v>
+      </c>
+      <c r="E4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="1">
-        <v>224</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="B5" s="3">
+        <v>0.524896681308746</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.80344200134277299</v>
+      </c>
+      <c r="D5">
+        <v>224</v>
+      </c>
+      <c r="E5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="1">
-        <v>224</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="B6" s="3">
+        <v>0.27091634273528997</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.90670287609100297</v>
+      </c>
+      <c r="D6">
+        <v>224</v>
+      </c>
+      <c r="E6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="1">
-        <v>224</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="B7" s="3">
+        <v>0.25743499398231501</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.90942031145095803</v>
+      </c>
+      <c r="D7">
+        <v>224</v>
+      </c>
+      <c r="E7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="1">
-        <v>224</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="B8" s="3">
+        <v>0.47506558895111001</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.82336956262588501</v>
+      </c>
+      <c r="D8">
+        <v>224</v>
+      </c>
+      <c r="E8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="1">
-        <v>224</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="B9" s="3">
+        <v>0.28164747357368403</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.90307968854904097</v>
+      </c>
+      <c r="D9">
+        <v>224</v>
+      </c>
+      <c r="E9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="1">
-        <v>224</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="B10" s="3">
+        <v>0.24787789583206099</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.92028987407684304</v>
+      </c>
+      <c r="D10">
+        <v>224</v>
+      </c>
+      <c r="E10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="1">
-        <v>224</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="B11" s="3">
+        <v>0.42793497443199102</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.85235506296157804</v>
+      </c>
+      <c r="D11">
+        <v>224</v>
+      </c>
+      <c r="E11" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
The models were newly trained.
</commit_message>
<xml_diff>
--- a/model_information/Performance By Model.xlsx
+++ b/model_information/Performance By Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyun\Desktop\RecycleWasteClassifier\model_information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B061018-30D4-41F9-94D6-D88E0DC69AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473E16CC-B700-43D9-8482-2A2A74184C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7065" yWindow="1380" windowWidth="17025" windowHeight="12930" xr2:uid="{3D546535-CEB8-4C73-9D93-428EFDA1FC9D}"/>
+    <workbookView xWindow="12735" yWindow="3390" windowWidth="12345" windowHeight="9795" xr2:uid="{3D546535-CEB8-4C73-9D93-428EFDA1FC9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -126,9 +126,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="0.000_ "/>
-    <numFmt numFmtId="178" formatCode="0.00_ "/>
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -176,11 +175,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -498,213 +497,203 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFAB712-2674-4A68-BC93-213602476CB7}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3">
-        <v>0.73988103866577104</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0.72463768720626798</v>
-      </c>
-      <c r="D2">
-        <v>224</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="B2" s="2">
+        <v>224</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.75434976816177302</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.71465969085693304</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3">
-        <v>0.45119205117225603</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.84601449966430597</v>
-      </c>
-      <c r="D3">
-        <v>224</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B3" s="2">
+        <v>224</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.34409651160240101</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.88132637739181496</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3">
-        <v>0.33470913767814597</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0.88949275016784601</v>
-      </c>
-      <c r="D4">
-        <v>224</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="B4" s="2">
+        <v>224</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.30661496520042397</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.89965093135833696</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3">
-        <v>0.524896681308746</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0.80344200134277299</v>
-      </c>
-      <c r="D5">
-        <v>224</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="B5" s="2">
+        <v>224</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>9</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.54651391506195002</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.791448533535003</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="3">
-        <v>0.27091634273528997</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0.90670287609100297</v>
-      </c>
-      <c r="D6">
-        <v>224</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="B6" s="2">
+        <v>224</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>12</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.29235821962356501</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.90663176774978604</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="3">
-        <v>0.25743499398231501</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0.90942031145095803</v>
-      </c>
-      <c r="D7">
-        <v>224</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="B7" s="2">
+        <v>224</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.30794841051101601</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.89790576696395796</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="3">
-        <v>0.47506558895111001</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0.82336956262588501</v>
-      </c>
-      <c r="D8">
-        <v>224</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="B8" s="2">
+        <v>224</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.52162706851959195</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.80715531110763505</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="3">
-        <v>0.28164747357368403</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0.90307968854904097</v>
-      </c>
-      <c r="D9">
-        <v>224</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="B9" s="2">
+        <v>224</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.35025388002395602</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.89267015457153298</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="3">
-        <v>0.24787789583206099</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0.92028987407684304</v>
-      </c>
-      <c r="D10">
-        <v>224</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="B10" s="2">
+        <v>224</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>23</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.25453931093215898</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.93019199371337802</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="3">
-        <v>0.42793497443199102</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0.85235506296157804</v>
-      </c>
-      <c r="D11">
-        <v>224</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="B11" s="2">
+        <v>224</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="D11" s="3">
+        <v>0.46997523307800199</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.83595114946365301</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>

</xml_diff>

<commit_message>
Modified the performance table of models.
</commit_message>
<xml_diff>
--- a/model_information/Performance By Model.xlsx
+++ b/model_information/Performance By Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyun\Desktop\RecycleWasteClassifier\model_information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473E16CC-B700-43D9-8482-2A2A74184C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA01D0B1-C9A7-4BDB-BC32-1BFDB88ED215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12735" yWindow="3390" windowWidth="12345" windowHeight="9795" xr2:uid="{3D546535-CEB8-4C73-9D93-428EFDA1FC9D}"/>
+    <workbookView xWindow="8730" yWindow="1740" windowWidth="12345" windowHeight="9795" xr2:uid="{3D546535-CEB8-4C73-9D93-428EFDA1FC9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -497,7 +497,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFAB712-2674-4A68-BC93-213602476CB7}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
The training data is organized and the model is ready for training.
</commit_message>
<xml_diff>
--- a/model_information/Performance By Model.xlsx
+++ b/model_information/Performance By Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyun\Desktop\RecycleWasteClassifier\model_information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA01D0B1-C9A7-4BDB-BC32-1BFDB88ED215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630248D8-962D-437C-B47A-BF79ED731627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8730" yWindow="1740" windowWidth="12345" windowHeight="9795" xr2:uid="{3D546535-CEB8-4C73-9D93-428EFDA1FC9D}"/>
   </bookViews>
@@ -495,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFAB712-2674-4A68-BC93-213602476CB7}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -510,7 +510,7 @@
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
@@ -524,7 +524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -534,14 +534,14 @@
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3">
+      <c r="F2" s="3">
         <v>0.75434976816177302</v>
       </c>
-      <c r="E2" s="3">
+      <c r="G2" s="3">
         <v>0.71465969085693304</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -551,14 +551,14 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3">
+      <c r="F3" s="3">
         <v>0.34409651160240101</v>
       </c>
-      <c r="E3" s="3">
+      <c r="G3" s="3">
         <v>0.88132637739181496</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -568,14 +568,14 @@
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3">
+      <c r="F4" s="3">
         <v>0.30661496520042397</v>
       </c>
-      <c r="E4" s="3">
+      <c r="G4" s="3">
         <v>0.89965093135833696</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -585,14 +585,14 @@
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="3">
+      <c r="F5" s="3">
         <v>0.54651391506195002</v>
       </c>
-      <c r="E5" s="3">
+      <c r="G5" s="3">
         <v>0.791448533535003</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -602,14 +602,14 @@
       <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="3">
+      <c r="F6" s="3">
         <v>0.29235821962356501</v>
       </c>
-      <c r="E6" s="3">
+      <c r="G6" s="3">
         <v>0.90663176774978604</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -619,14 +619,14 @@
       <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="3">
+      <c r="F7" s="3">
         <v>0.30794841051101601</v>
       </c>
-      <c r="E7" s="3">
+      <c r="G7" s="3">
         <v>0.89790576696395796</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -636,14 +636,14 @@
       <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="3">
+      <c r="F8" s="3">
         <v>0.52162706851959195</v>
       </c>
-      <c r="E8" s="3">
+      <c r="G8" s="3">
         <v>0.80715531110763505</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -653,14 +653,14 @@
       <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="3">
+      <c r="F9" s="3">
         <v>0.35025388002395602</v>
       </c>
-      <c r="E9" s="3">
+      <c r="G9" s="3">
         <v>0.89267015457153298</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -670,14 +670,14 @@
       <c r="C10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="3">
+      <c r="F10" s="3">
         <v>0.25453931093215898</v>
       </c>
-      <c r="E10" s="3">
+      <c r="G10" s="3">
         <v>0.93019199371337802</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -687,14 +687,14 @@
       <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="3">
+      <c r="F11" s="3">
         <v>0.46997523307800199</v>
       </c>
-      <c r="E11" s="3">
+      <c r="G11" s="3">
         <v>0.83595114946365301</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>

</xml_diff>

<commit_message>
Train the models anew and save the artifacts.
</commit_message>
<xml_diff>
--- a/model_information/Performance By Model.xlsx
+++ b/model_information/Performance By Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyun\Desktop\RecycleWasteClassifier\model_information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630248D8-962D-437C-B47A-BF79ED731627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953C6563-77CD-495E-BF22-5A54AB35D63D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8730" yWindow="1740" windowWidth="12345" windowHeight="9795" xr2:uid="{3D546535-CEB8-4C73-9D93-428EFDA1FC9D}"/>
+    <workbookView xWindow="11940" yWindow="2295" windowWidth="13470" windowHeight="11145" xr2:uid="{3D546535-CEB8-4C73-9D93-428EFDA1FC9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -498,7 +498,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -508,6 +508,7 @@
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="5.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -534,12 +535,14 @@
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="3">
-        <v>0.75434976816177302</v>
-      </c>
-      <c r="G2" s="3">
-        <v>0.71465969085693304</v>
-      </c>
+      <c r="D2" s="3">
+        <v>0.72960686683654696</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.72545754909515303</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -551,12 +554,14 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="3">
-        <v>0.34409651160240101</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0.88132637739181496</v>
-      </c>
+      <c r="D3" s="3">
+        <v>0.38250002264976501</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.87104827165603604</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -568,12 +573,14 @@
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="3">
-        <v>0.30661496520042397</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0.89965093135833696</v>
-      </c>
+      <c r="D4" s="3">
+        <v>0.364557415246963</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.87437605857849099</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -585,12 +592,14 @@
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="3">
-        <v>0.54651391506195002</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0.791448533535003</v>
-      </c>
+      <c r="D5" s="3">
+        <v>0.582988440990448</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.78702163696288996</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -602,12 +611,14 @@
       <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="3">
-        <v>0.29235821962356501</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0.90663176774978604</v>
-      </c>
+      <c r="D6" s="3">
+        <v>0.30606013536453203</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.89767056703567505</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -619,12 +630,14 @@
       <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="3">
-        <v>0.30794841051101601</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0.89790576696395796</v>
-      </c>
+      <c r="D7" s="3">
+        <v>0.37662041187286299</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.87687188386917103</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -636,12 +649,14 @@
       <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="3">
-        <v>0.52162706851959195</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0.80715531110763505</v>
-      </c>
+      <c r="D8" s="3">
+        <v>0.53930389881134</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.80782032012939398</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -653,12 +668,14 @@
       <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="3">
-        <v>0.35025388002395602</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0.89267015457153298</v>
-      </c>
+      <c r="D9" s="3">
+        <v>0.32160222530364901</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.90432614088058405</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -670,12 +687,14 @@
       <c r="C10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="3">
-        <v>0.25453931093215898</v>
-      </c>
-      <c r="G10" s="3">
-        <v>0.93019199371337802</v>
-      </c>
+      <c r="D10" s="3">
+        <v>0.295376986265182</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.91763728857040405</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -687,12 +706,14 @@
       <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="3">
-        <v>0.46997523307800199</v>
-      </c>
-      <c r="G11" s="3">
-        <v>0.83595114946365301</v>
-      </c>
+      <c r="D11" s="3">
+        <v>0.49054548144340498</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.83028286695480302</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>

</xml_diff>